<commit_message>
more edits to introduction
</commit_message>
<xml_diff>
--- a/docs/literature/Age5BPERAdjustments.xlsx
+++ b/docs/literature/Age5BPERAdjustments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/angelika_hagen-breaux_dfw_wa_gov/Documents/Documents/Calibration/2014NewBasePeriod/Documentation/fram_doc/literature/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angelika\Documents\CalibDoc\CalibDoc\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{E3D78ED0-3A64-43E4-B25A-B107524B620A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F38E32EA-C67B-4AC3-A1AA-6C1A383C3041}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10279AEB-6503-4A6C-ABBB-3C24A3EDD1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{118B8A05-A168-4396-BAA9-3636F21A3067}"/>
   </bookViews>
@@ -16,21 +16,10 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1180,7 +1169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1290,9 +1279,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1610,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49814D49-383A-4A40-9082-9E147D337DF3}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,79 +1608,107 @@
     <col min="5" max="5" width="6.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+    <row r="1" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G1" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I1" s="35" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="2">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12">
+        <v>1</v>
+      </c>
+      <c r="G2" s="29">
+        <v>4</v>
+      </c>
+      <c r="H2" s="36">
+        <v>0.13450000000000001</v>
+      </c>
+      <c r="I2" s="31">
+        <v>5.8999999999999997E-2</v>
+      </c>
+    </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2">
-        <v>3</v>
-      </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="29">
-        <v>4</v>
-      </c>
-      <c r="H3" s="36">
-        <v>0.13450000000000001</v>
-      </c>
-      <c r="I3" s="31">
-        <v>5.8999999999999997E-2</v>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>6</v>
+      </c>
+      <c r="G3" s="5">
+        <v>10</v>
+      </c>
+      <c r="H3" s="37">
+        <v>0.35830000000000001</v>
+      </c>
+      <c r="I3" s="32">
+        <v>6.7699999999999996E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="39">
-        <v>1</v>
-      </c>
-      <c r="D4" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="4">
         <v>1</v>
       </c>
       <c r="F4" s="3">
@@ -1712,76 +1726,76 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5" s="39">
-        <v>1</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="39">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="4">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="4">
         <v>1</v>
       </c>
       <c r="F5" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G5" s="5">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H5" s="37">
-        <v>0.35830000000000001</v>
+        <v>0.18290000000000001</v>
       </c>
       <c r="I5" s="32">
-        <v>6.7699999999999996E-2</v>
+        <v>4.6399999999999997E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>9</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="C6" s="39">
-        <v>15</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="39">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="4">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
       </c>
       <c r="G6" s="5">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H6" s="37">
-        <v>0.18290000000000001</v>
+        <v>0.38869999999999999</v>
       </c>
       <c r="I6" s="32">
-        <v>4.6399999999999997E-2</v>
+        <v>1.06E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>10</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C7" s="39">
-        <v>13</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="39">
+      <c r="C7" s="4">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="4">
         <v>2</v>
       </c>
       <c r="F7" s="3">
@@ -1791,27 +1805,27 @@
         <v>0</v>
       </c>
       <c r="H7" s="37">
-        <v>0.38869999999999999</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="I7" s="32">
-        <v>1.06E-2</v>
+        <v>1.8499999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>10</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C8" s="39">
-        <v>15</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="39">
-        <v>2</v>
+      <c r="C8" s="4">
+        <v>36</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
@@ -1820,56 +1834,56 @@
         <v>0</v>
       </c>
       <c r="H8" s="37">
-        <v>0.26100000000000001</v>
+        <v>0.17349999999999999</v>
       </c>
       <c r="I8" s="32">
-        <v>1.8499999999999999E-2</v>
+        <v>7.7299999999999994E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>10</v>
-      </c>
-      <c r="B9" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="39">
-        <v>36</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="39">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="4">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2</v>
       </c>
       <c r="F9" s="3">
         <v>1</v>
       </c>
       <c r="G9" s="5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H9" s="37">
-        <v>0.17349999999999999</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="I9" s="32">
-        <v>7.7299999999999994E-2</v>
+        <v>9.5600000000000004E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>17</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C10" s="39">
-        <v>10</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="39">
-        <v>2</v>
+      <c r="C10" s="4">
+        <v>42</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
@@ -1878,101 +1892,72 @@
         <v>9</v>
       </c>
       <c r="H10" s="37">
-        <v>0.29399999999999998</v>
+        <v>0.2301</v>
       </c>
       <c r="I10" s="32">
-        <v>9.5600000000000004E-2</v>
+        <v>2.6100000000000002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>17</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>189</v>
-      </c>
-      <c r="C11" s="39">
-        <v>42</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" s="39">
-        <v>3</v>
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" s="4">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H11" s="37">
-        <v>0.2301</v>
+        <v>0.3896</v>
       </c>
       <c r="I11" s="32">
-        <v>2.6100000000000002E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>22</v>
-      </c>
-      <c r="B12" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="C12" s="39">
-        <v>10</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="39">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1</v>
-      </c>
-      <c r="G12" s="5">
+        <v>6.7900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <v>35</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C12" s="6">
+        <v>34</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="G12" s="8">
         <v>0</v>
       </c>
-      <c r="H12" s="37">
-        <v>0.3896</v>
-      </c>
-      <c r="I12" s="32">
-        <v>6.7900000000000002E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7">
-        <v>35</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C13" s="6">
-        <v>34</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-      <c r="H13" s="38">
+      <c r="H12" s="38">
         <v>0.65090000000000003</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I12" s="33">
         <v>0.13639999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>